<commit_message>
Added util files, Need to correct slashChanger
</commit_message>
<xml_diff>
--- a/src/test/resources/Test.xlsx
+++ b/src/test/resources/Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="8175"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>TestCase</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>PageTitle</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>N</t>
@@ -136,7 +133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -171,7 +168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,7 +410,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pass testdata from json File
</commit_message>
<xml_diff>
--- a/src/test/resources/Test.xlsx
+++ b/src/test/resources/Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="8175"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>TestCase</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,7 +174,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,6 +419,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re run failed testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/Test.xlsx
+++ b/src/test/resources/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="8175" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="RunModes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>TestCase</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>PageTitle</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Y</t>
@@ -452,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,10 +485,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -514,87 +511,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -610,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>